<commit_message>
Fix lỗi time VNPAY lúc deploy
</commit_message>
<xml_diff>
--- a/src/main/resources/template/report/Bao_cao_tong_ket_khuyen_mai.xlsx
+++ b/src/main/resources/template/report/Bao_cao_tong_ket_khuyen_mai.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E1E768-1A72-495F-A6A6-D550926AB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434B99C8-B425-41FA-81C3-B47EF68257F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="19440" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Báo cáo doanh thu theo hãng xe" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>&lt;jx:forEach items="${lstData}" var="vo" varStatus="status"&gt;</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>${vo.promotionTDate}</t>
+  </si>
+  <si>
+    <t>${vo.ticketPrice}</t>
+  </si>
+  <si>
+    <t>${vo.revenue}</t>
+  </si>
+  <si>
+    <t>Số tiền trước CK</t>
+  </si>
+  <si>
+    <t>Doanh thu sau CK</t>
   </si>
 </sst>
 </file>
@@ -274,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -324,9 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -682,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:R12"/>
+  <dimension ref="A4:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -695,22 +704,22 @@
     <col min="3" max="3" width="27.109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" style="4" customWidth="1"/>
     <col min="5" max="5" width="17" style="4" customWidth="1"/>
-    <col min="6" max="7" width="21" style="4" customWidth="1"/>
-    <col min="8" max="8" width="27.21875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16" style="4" customWidth="1"/>
-    <col min="10" max="10" width="23.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" style="4" customWidth="1"/>
-    <col min="12" max="14" width="20.33203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="14.77734375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="34" style="4" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="4"/>
+    <col min="6" max="9" width="21" style="4" customWidth="1"/>
+    <col min="10" max="10" width="27.21875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="4" customWidth="1"/>
+    <col min="14" max="16" width="20.33203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="34" style="4" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
     </row>
-    <row r="5" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
@@ -720,9 +729,9 @@
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -730,8 +739,10 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
@@ -747,9 +758,9 @@
       <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -757,8 +768,10 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -766,8 +779,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -775,8 +788,10 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -798,8 +813,12 @@
       <c r="G8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="H8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -809,8 +828,10 @@
       <c r="P8"/>
       <c r="Q8"/>
       <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
     </row>
-    <row r="9" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
@@ -820,19 +841,21 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9" s="14"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9"/>
       <c r="K9"/>
-      <c r="L9"/>
+      <c r="L9" s="14"/>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
     </row>
-    <row r="10" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
@@ -851,11 +874,15 @@
       <c r="F10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H10"/>
-      <c r="I10"/>
+      <c r="H10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -865,8 +892,10 @@
       <c r="P10"/>
       <c r="Q10"/>
       <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
     </row>
-    <row r="11" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -876,27 +905,29 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11"/>
       <c r="K11"/>
-      <c r="L11"/>
+      <c r="L11" s="14"/>
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
     </row>
-    <row r="12" spans="1:18" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -906,6 +937,8 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>